<commit_message>
Updated February 22, 2021.
</commit_message>
<xml_diff>
--- a/wrangle/data/interventions/standardized-restrictions.xlsx
+++ b/wrangle/data/interventions/standardized-restrictions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kt/Documents/work/STATCAN/Projects/nick/CovidTimeline/wrangle/data/interventions/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D68821DA-88F3-0D45-9B91-442D8AD0E4B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{198C65F6-A980-874D-AB38-A75B877DD4EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1960" yWindow="2060" windowWidth="26840" windowHeight="15940" activeTab="2" xr2:uid="{86546001-3EFC-E246-8DB8-6E829CCD7EB6}"/>
+    <workbookView xWindow="1960" yWindow="2060" windowWidth="26840" windowHeight="15940" activeTab="1" xr2:uid="{86546001-3EFC-E246-8DB8-6E829CCD7EB6}"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="1" r:id="rId1"/>
@@ -119,9 +119,6 @@
     <t>https://www.quebec.ca/en/health/health-issues/a-z/2019-coronavirus/progressive-regional-alert-and-intervention-system/</t>
   </si>
   <si>
-    <t>Limits to operations such as nightclubs restricted to operate as restaurants, establishments obligated to reduced hours of operation, or partial closures.</t>
-  </si>
-  <si>
     <t>Green level</t>
   </si>
   <si>
@@ -144,6 +141,9 @@
   </si>
   <si>
     <t>https://www2.gnb.ca/content/dam/gnb/Departments/eco-bce/Promo/covid-19/red-phase-frequently-asked-questions.pdf</t>
+  </si>
+  <si>
+    <t>Limits to operations such as nightclubs restricted to operate as restaurants, establishments obligated to reduced hours of operation or number of guests, or partial closures.</t>
   </si>
 </sst>
 </file>
@@ -902,16 +902,16 @@
         <v>26</v>
       </c>
       <c r="K2" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="L2" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="L2" s="16" t="s">
+      <c r="M2" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="M2" s="17" t="s">
+      <c r="N2" s="20" t="s">
         <v>31</v>
-      </c>
-      <c r="N2" s="20" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="3" spans="1:14">
@@ -1175,7 +1175,7 @@
         <v>18</v>
       </c>
       <c r="N8" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:14">
@@ -1368,8 +1368,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7501E192-E645-FE48-AF98-C21D02C07D3A}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1379,7 +1379,7 @@
         <v>17</v>
       </c>
       <c r="B1" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -1387,7 +1387,7 @@
         <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1407,7 +1407,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EABBA44-C292-CB4F-B560-29A615710003}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -1437,10 +1437,10 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>